<commit_message>
validate now ignores when dao files are not present, as Hyrax uris are now uploaded at a later stage
</commit_message>
<xml_diff>
--- a/asInventory.xlsx
+++ b/asInventory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\asInventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gw234478\win\asInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -511,7 +511,7 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" activeCellId="1" sqref="I17 F4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>